<commit_message>
Update download sample file
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/upload/UserUploadTemplate.xlsx
+++ b/src/main/resources/templates/upload/UserUploadTemplate.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Nguyen Duc</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>vi</t>
   </si>
@@ -75,7 +72,16 @@
     <t>nguyenducmanh2581911@gmail.com</t>
   </si>
   <si>
-    <t>catched_bitch</t>
+    <t>user_login</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>CN</t>
   </si>
 </sst>
 </file>
@@ -429,7 +435,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,46 +449,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -493,22 +499,40 @@
         <v>10333</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
         <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Upload, Download file sample, create user
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/upload/UserUploadTemplate.xlsx
+++ b/src/main/resources/templates/upload/UserUploadTemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>vi</t>
   </si>
@@ -54,9 +54,6 @@
     <t>STT</t>
   </si>
   <si>
-    <t>ownID *</t>
-  </si>
-  <si>
     <t>login *</t>
   </si>
   <si>
@@ -69,12 +66,6 @@
     <t>0886306155666</t>
   </si>
   <si>
-    <t>nguyenducmanh2581911@gmail.com</t>
-  </si>
-  <si>
-    <t>user_login</t>
-  </si>
-  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -82,6 +73,12 @@
   </si>
   <si>
     <t>CN</t>
+  </si>
+  <si>
+    <t>nguyenducmanh2581911@gmail.comz</t>
+  </si>
+  <si>
+    <t>user_loginm</t>
   </si>
 </sst>
 </file>
@@ -432,22 +429,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="36.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -455,89 +452,83 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>10333</v>
+      <c r="B2" t="s">
+        <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>